<commit_message>
added files, screenshot, and recording
</commit_message>
<xml_diff>
--- a/Final Project/data/use_pet_capita.xlsx
+++ b/Final Project/data/use_pet_capita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wwwdev\website\state\seds\sep_sum\html\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellelouie/Documents/Berkeley/2024-2025/STAT 198/stat-198/Final Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D0AE3B-2C48-4E7D-B038-1D0154F60B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0874D2BD-AFF2-964A-8653-3A4AB5D9393D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" tabRatio="657" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="14980" tabRatio="657" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="7" r:id="rId1"/>
@@ -1328,44 +1328,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.19921875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="43.8984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="38.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" customWidth="1"/>
     <col min="4" max="4" width="9" style="4"/>
     <col min="5" max="5" width="9.5" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
@@ -1450,25 +1450,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
@@ -1499,24 +1499,24 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="11" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="64" width="11.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="11" customWidth="1"/>
+    <col min="3" max="6" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="64" width="11.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="65" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1941,7 +1941,7 @@
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -2172,7 +2172,7 @@
       <c r="CV5" s="10"/>
       <c r="CW5" s="10"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -2403,7 +2403,7 @@
       <c r="CV6" s="10"/>
       <c r="CW6" s="10"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
@@ -2634,7 +2634,7 @@
       <c r="CV7" s="10"/>
       <c r="CW7" s="10"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -2865,7 +2865,7 @@
       <c r="CV8" s="10"/>
       <c r="CW8" s="10"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="CV9" s="10"/>
       <c r="CW9" s="10"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -3327,7 +3327,7 @@
       <c r="CV10" s="10"/>
       <c r="CW10" s="10"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>37</v>
       </c>
@@ -3558,7 +3558,7 @@
       <c r="CV11" s="10"/>
       <c r="CW11" s="10"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="CV12" s="10"/>
       <c r="CW12" s="10"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -4020,7 +4020,7 @@
       <c r="CV13" s="10"/>
       <c r="CW13" s="10"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>40</v>
       </c>
@@ -4251,7 +4251,7 @@
       <c r="CV14" s="10"/>
       <c r="CW14" s="10"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
@@ -4482,7 +4482,7 @@
       <c r="CV15" s="10"/>
       <c r="CW15" s="10"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -4713,7 +4713,7 @@
       <c r="CV16" s="10"/>
       <c r="CW16" s="10"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
@@ -4944,7 +4944,7 @@
       <c r="CV17" s="10"/>
       <c r="CW17" s="10"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>44</v>
       </c>
@@ -5175,7 +5175,7 @@
       <c r="CV18" s="10"/>
       <c r="CW18" s="10"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -5406,7 +5406,7 @@
       <c r="CV19" s="10"/>
       <c r="CW19" s="10"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -5637,7 +5637,7 @@
       <c r="CV20" s="10"/>
       <c r="CW20" s="10"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
@@ -5868,7 +5868,7 @@
       <c r="CV21" s="10"/>
       <c r="CW21" s="10"/>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
@@ -6099,7 +6099,7 @@
       <c r="CV22" s="10"/>
       <c r="CW22" s="10"/>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>49</v>
       </c>
@@ -6330,7 +6330,7 @@
       <c r="CV23" s="10"/>
       <c r="CW23" s="10"/>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
@@ -6561,7 +6561,7 @@
       <c r="CV24" s="10"/>
       <c r="CW24" s="10"/>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
@@ -6792,7 +6792,7 @@
       <c r="CV25" s="10"/>
       <c r="CW25" s="10"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>52</v>
       </c>
@@ -7023,7 +7023,7 @@
       <c r="CV26" s="10"/>
       <c r="CW26" s="10"/>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
@@ -7254,7 +7254,7 @@
       <c r="CV27" s="10"/>
       <c r="CW27" s="10"/>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>54</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="CV28" s="10"/>
       <c r="CW28" s="10"/>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>55</v>
       </c>
@@ -7716,7 +7716,7 @@
       <c r="CV29" s="10"/>
       <c r="CW29" s="10"/>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>56</v>
       </c>
@@ -7947,7 +7947,7 @@
       <c r="CV30" s="10"/>
       <c r="CW30" s="10"/>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>57</v>
       </c>
@@ -8178,7 +8178,7 @@
       <c r="CV31" s="10"/>
       <c r="CW31" s="10"/>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>58</v>
       </c>
@@ -8409,7 +8409,7 @@
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>59</v>
       </c>
@@ -8640,7 +8640,7 @@
       <c r="CV33" s="10"/>
       <c r="CW33" s="10"/>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>60</v>
       </c>
@@ -8871,7 +8871,7 @@
       <c r="CV34" s="10"/>
       <c r="CW34" s="10"/>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>61</v>
       </c>
@@ -9102,7 +9102,7 @@
       <c r="CV35" s="10"/>
       <c r="CW35" s="10"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>62</v>
       </c>
@@ -9333,7 +9333,7 @@
       <c r="CV36" s="10"/>
       <c r="CW36" s="10"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
@@ -9564,7 +9564,7 @@
       <c r="CV37" s="10"/>
       <c r="CW37" s="10"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>64</v>
       </c>
@@ -9795,7 +9795,7 @@
       <c r="CV38" s="10"/>
       <c r="CW38" s="10"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -10026,7 +10026,7 @@
       <c r="CV39" s="10"/>
       <c r="CW39" s="10"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>66</v>
       </c>
@@ -10257,7 +10257,7 @@
       <c r="CV40" s="10"/>
       <c r="CW40" s="10"/>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>67</v>
       </c>
@@ -10488,7 +10488,7 @@
       <c r="CV41" s="10"/>
       <c r="CW41" s="10"/>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>68</v>
       </c>
@@ -10719,7 +10719,7 @@
       <c r="CV42" s="10"/>
       <c r="CW42" s="10"/>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>69</v>
       </c>
@@ -10950,7 +10950,7 @@
       <c r="CV43" s="10"/>
       <c r="CW43" s="10"/>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>70</v>
       </c>
@@ -11181,7 +11181,7 @@
       <c r="CV44" s="10"/>
       <c r="CW44" s="10"/>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>71</v>
       </c>
@@ -11412,7 +11412,7 @@
       <c r="CV45" s="10"/>
       <c r="CW45" s="10"/>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>72</v>
       </c>
@@ -11643,7 +11643,7 @@
       <c r="CV46" s="10"/>
       <c r="CW46" s="10"/>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>73</v>
       </c>
@@ -11874,7 +11874,7 @@
       <c r="CV47" s="10"/>
       <c r="CW47" s="10"/>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>74</v>
       </c>
@@ -12105,7 +12105,7 @@
       <c r="CV48" s="10"/>
       <c r="CW48" s="10"/>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>75</v>
       </c>
@@ -12336,7 +12336,7 @@
       <c r="CV49" s="10"/>
       <c r="CW49" s="10"/>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>76</v>
       </c>
@@ -12567,7 +12567,7 @@
       <c r="CV50" s="10"/>
       <c r="CW50" s="10"/>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>77</v>
       </c>
@@ -12798,7 +12798,7 @@
       <c r="CV51" s="10"/>
       <c r="CW51" s="10"/>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>78</v>
       </c>
@@ -13029,7 +13029,7 @@
       <c r="CV52" s="10"/>
       <c r="CW52" s="10"/>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>79</v>
       </c>
@@ -13260,7 +13260,7 @@
       <c r="CV53" s="10"/>
       <c r="CW53" s="10"/>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>80</v>
       </c>
@@ -13491,7 +13491,7 @@
       <c r="CV54" s="10"/>
       <c r="CW54" s="10"/>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>81</v>
       </c>
@@ -13722,7 +13722,7 @@
       <c r="CV55" s="10"/>
       <c r="CW55" s="10"/>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -13802,7 +13802,7 @@
       <c r="BZ56" s="9"/>
       <c r="CA56" s="9"/>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -13882,7 +13882,7 @@
       <c r="BZ57" s="9"/>
       <c r="CA57" s="9"/>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -13962,7 +13962,7 @@
       <c r="BZ58" s="9"/>
       <c r="CA58" s="9"/>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -14042,7 +14042,7 @@
       <c r="BZ59" s="9"/>
       <c r="CA59" s="9"/>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -14139,24 +14139,24 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="11" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="64" width="11.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="11" customWidth="1"/>
+    <col min="3" max="6" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="64" width="11.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="65" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -14350,7 +14350,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -14581,7 +14581,7 @@
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -14812,7 +14812,7 @@
       <c r="CV5" s="10"/>
       <c r="CW5" s="10"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -15043,7 +15043,7 @@
       <c r="CV6" s="10"/>
       <c r="CW6" s="10"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
@@ -15274,7 +15274,7 @@
       <c r="CV7" s="10"/>
       <c r="CW7" s="10"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -15505,7 +15505,7 @@
       <c r="CV8" s="10"/>
       <c r="CW8" s="10"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -15736,7 +15736,7 @@
       <c r="CV9" s="10"/>
       <c r="CW9" s="10"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -15967,7 +15967,7 @@
       <c r="CV10" s="10"/>
       <c r="CW10" s="10"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>37</v>
       </c>
@@ -16198,7 +16198,7 @@
       <c r="CV11" s="10"/>
       <c r="CW11" s="10"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
@@ -16429,7 +16429,7 @@
       <c r="CV12" s="10"/>
       <c r="CW12" s="10"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -16660,7 +16660,7 @@
       <c r="CV13" s="10"/>
       <c r="CW13" s="10"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>40</v>
       </c>
@@ -16891,7 +16891,7 @@
       <c r="CV14" s="10"/>
       <c r="CW14" s="10"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
@@ -17122,7 +17122,7 @@
       <c r="CV15" s="10"/>
       <c r="CW15" s="10"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -17353,7 +17353,7 @@
       <c r="CV16" s="10"/>
       <c r="CW16" s="10"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
@@ -17584,7 +17584,7 @@
       <c r="CV17" s="10"/>
       <c r="CW17" s="10"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>44</v>
       </c>
@@ -17815,7 +17815,7 @@
       <c r="CV18" s="10"/>
       <c r="CW18" s="10"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -18046,7 +18046,7 @@
       <c r="CV19" s="10"/>
       <c r="CW19" s="10"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -18277,7 +18277,7 @@
       <c r="CV20" s="10"/>
       <c r="CW20" s="10"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
@@ -18508,7 +18508,7 @@
       <c r="CV21" s="10"/>
       <c r="CW21" s="10"/>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
@@ -18739,7 +18739,7 @@
       <c r="CV22" s="10"/>
       <c r="CW22" s="10"/>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>49</v>
       </c>
@@ -18970,7 +18970,7 @@
       <c r="CV23" s="10"/>
       <c r="CW23" s="10"/>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
@@ -19201,7 +19201,7 @@
       <c r="CV24" s="10"/>
       <c r="CW24" s="10"/>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
@@ -19432,7 +19432,7 @@
       <c r="CV25" s="10"/>
       <c r="CW25" s="10"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>52</v>
       </c>
@@ -19663,7 +19663,7 @@
       <c r="CV26" s="10"/>
       <c r="CW26" s="10"/>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
@@ -19894,7 +19894,7 @@
       <c r="CV27" s="10"/>
       <c r="CW27" s="10"/>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>54</v>
       </c>
@@ -20125,7 +20125,7 @@
       <c r="CV28" s="10"/>
       <c r="CW28" s="10"/>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>55</v>
       </c>
@@ -20356,7 +20356,7 @@
       <c r="CV29" s="10"/>
       <c r="CW29" s="10"/>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>56</v>
       </c>
@@ -20587,7 +20587,7 @@
       <c r="CV30" s="10"/>
       <c r="CW30" s="10"/>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>57</v>
       </c>
@@ -20818,7 +20818,7 @@
       <c r="CV31" s="10"/>
       <c r="CW31" s="10"/>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>58</v>
       </c>
@@ -21049,7 +21049,7 @@
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>59</v>
       </c>
@@ -21280,7 +21280,7 @@
       <c r="CV33" s="10"/>
       <c r="CW33" s="10"/>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>60</v>
       </c>
@@ -21511,7 +21511,7 @@
       <c r="CV34" s="10"/>
       <c r="CW34" s="10"/>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>61</v>
       </c>
@@ -21742,7 +21742,7 @@
       <c r="CV35" s="10"/>
       <c r="CW35" s="10"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>62</v>
       </c>
@@ -21973,7 +21973,7 @@
       <c r="CV36" s="10"/>
       <c r="CW36" s="10"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
@@ -22204,7 +22204,7 @@
       <c r="CV37" s="10"/>
       <c r="CW37" s="10"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>64</v>
       </c>
@@ -22435,7 +22435,7 @@
       <c r="CV38" s="10"/>
       <c r="CW38" s="10"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -22666,7 +22666,7 @@
       <c r="CV39" s="10"/>
       <c r="CW39" s="10"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>66</v>
       </c>
@@ -22897,7 +22897,7 @@
       <c r="CV40" s="10"/>
       <c r="CW40" s="10"/>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>67</v>
       </c>
@@ -23128,7 +23128,7 @@
       <c r="CV41" s="10"/>
       <c r="CW41" s="10"/>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>68</v>
       </c>
@@ -23359,7 +23359,7 @@
       <c r="CV42" s="10"/>
       <c r="CW42" s="10"/>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>69</v>
       </c>
@@ -23590,7 +23590,7 @@
       <c r="CV43" s="10"/>
       <c r="CW43" s="10"/>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>70</v>
       </c>
@@ -23821,7 +23821,7 @@
       <c r="CV44" s="10"/>
       <c r="CW44" s="10"/>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>71</v>
       </c>
@@ -24052,7 +24052,7 @@
       <c r="CV45" s="10"/>
       <c r="CW45" s="10"/>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>72</v>
       </c>
@@ -24283,7 +24283,7 @@
       <c r="CV46" s="10"/>
       <c r="CW46" s="10"/>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>73</v>
       </c>
@@ -24514,7 +24514,7 @@
       <c r="CV47" s="10"/>
       <c r="CW47" s="10"/>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>74</v>
       </c>
@@ -24745,7 +24745,7 @@
       <c r="CV48" s="10"/>
       <c r="CW48" s="10"/>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>75</v>
       </c>
@@ -24976,7 +24976,7 @@
       <c r="CV49" s="10"/>
       <c r="CW49" s="10"/>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>76</v>
       </c>
@@ -25207,7 +25207,7 @@
       <c r="CV50" s="10"/>
       <c r="CW50" s="10"/>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>77</v>
       </c>
@@ -25438,7 +25438,7 @@
       <c r="CV51" s="10"/>
       <c r="CW51" s="10"/>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>78</v>
       </c>
@@ -25669,7 +25669,7 @@
       <c r="CV52" s="10"/>
       <c r="CW52" s="10"/>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>79</v>
       </c>
@@ -25900,7 +25900,7 @@
       <c r="CV53" s="10"/>
       <c r="CW53" s="10"/>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>80</v>
       </c>
@@ -26131,7 +26131,7 @@
       <c r="CV54" s="10"/>
       <c r="CW54" s="10"/>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>81</v>
       </c>
@@ -26362,7 +26362,7 @@
       <c r="CV55" s="10"/>
       <c r="CW55" s="10"/>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -26442,7 +26442,7 @@
       <c r="BZ56" s="9"/>
       <c r="CA56" s="9"/>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -26522,7 +26522,7 @@
       <c r="BZ57" s="9"/>
       <c r="CA57" s="9"/>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -26602,7 +26602,7 @@
       <c r="BZ58" s="9"/>
       <c r="CA58" s="9"/>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -26682,7 +26682,7 @@
       <c r="BZ59" s="9"/>
       <c r="CA59" s="9"/>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -26778,23 +26778,23 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="6" customWidth="1"/>
-    <col min="2" max="6" width="11.3984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="64" width="11.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="6" customWidth="1"/>
+    <col min="2" max="6" width="11.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="64" width="11.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="65" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -26988,7 +26988,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -27219,7 +27219,7 @@
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -27450,7 +27450,7 @@
       <c r="CV5" s="10"/>
       <c r="CW5" s="10"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -27681,7 +27681,7 @@
       <c r="CV6" s="10"/>
       <c r="CW6" s="10"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
@@ -27912,7 +27912,7 @@
       <c r="CV7" s="10"/>
       <c r="CW7" s="10"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -28143,7 +28143,7 @@
       <c r="CV8" s="10"/>
       <c r="CW8" s="10"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -28374,7 +28374,7 @@
       <c r="CV9" s="10"/>
       <c r="CW9" s="10"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -28605,7 +28605,7 @@
       <c r="CV10" s="10"/>
       <c r="CW10" s="10"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>37</v>
       </c>
@@ -28836,7 +28836,7 @@
       <c r="CV11" s="10"/>
       <c r="CW11" s="10"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
@@ -29067,7 +29067,7 @@
       <c r="CV12" s="10"/>
       <c r="CW12" s="10"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -29298,7 +29298,7 @@
       <c r="CV13" s="10"/>
       <c r="CW13" s="10"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>40</v>
       </c>
@@ -29529,7 +29529,7 @@
       <c r="CV14" s="10"/>
       <c r="CW14" s="10"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
@@ -29760,7 +29760,7 @@
       <c r="CV15" s="10"/>
       <c r="CW15" s="10"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -29991,7 +29991,7 @@
       <c r="CV16" s="10"/>
       <c r="CW16" s="10"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
@@ -30222,7 +30222,7 @@
       <c r="CV17" s="10"/>
       <c r="CW17" s="10"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>44</v>
       </c>
@@ -30453,7 +30453,7 @@
       <c r="CV18" s="10"/>
       <c r="CW18" s="10"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -30684,7 +30684,7 @@
       <c r="CV19" s="10"/>
       <c r="CW19" s="10"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -30915,7 +30915,7 @@
       <c r="CV20" s="10"/>
       <c r="CW20" s="10"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
@@ -31146,7 +31146,7 @@
       <c r="CV21" s="10"/>
       <c r="CW21" s="10"/>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
@@ -31377,7 +31377,7 @@
       <c r="CV22" s="10"/>
       <c r="CW22" s="10"/>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>49</v>
       </c>
@@ -31608,7 +31608,7 @@
       <c r="CV23" s="10"/>
       <c r="CW23" s="10"/>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
@@ -31839,7 +31839,7 @@
       <c r="CV24" s="10"/>
       <c r="CW24" s="10"/>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
@@ -32070,7 +32070,7 @@
       <c r="CV25" s="10"/>
       <c r="CW25" s="10"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>52</v>
       </c>
@@ -32301,7 +32301,7 @@
       <c r="CV26" s="10"/>
       <c r="CW26" s="10"/>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
@@ -32532,7 +32532,7 @@
       <c r="CV27" s="10"/>
       <c r="CW27" s="10"/>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>54</v>
       </c>
@@ -32763,7 +32763,7 @@
       <c r="CV28" s="10"/>
       <c r="CW28" s="10"/>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>55</v>
       </c>
@@ -32994,7 +32994,7 @@
       <c r="CV29" s="10"/>
       <c r="CW29" s="10"/>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>56</v>
       </c>
@@ -33225,7 +33225,7 @@
       <c r="CV30" s="10"/>
       <c r="CW30" s="10"/>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>57</v>
       </c>
@@ -33456,7 +33456,7 @@
       <c r="CV31" s="10"/>
       <c r="CW31" s="10"/>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>58</v>
       </c>
@@ -33687,7 +33687,7 @@
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>59</v>
       </c>
@@ -33918,7 +33918,7 @@
       <c r="CV33" s="10"/>
       <c r="CW33" s="10"/>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>60</v>
       </c>
@@ -34149,7 +34149,7 @@
       <c r="CV34" s="10"/>
       <c r="CW34" s="10"/>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>61</v>
       </c>
@@ -34380,7 +34380,7 @@
       <c r="CV35" s="10"/>
       <c r="CW35" s="10"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>62</v>
       </c>
@@ -34611,7 +34611,7 @@
       <c r="CV36" s="10"/>
       <c r="CW36" s="10"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
@@ -34842,7 +34842,7 @@
       <c r="CV37" s="10"/>
       <c r="CW37" s="10"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>64</v>
       </c>
@@ -35073,7 +35073,7 @@
       <c r="CV38" s="10"/>
       <c r="CW38" s="10"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -35304,7 +35304,7 @@
       <c r="CV39" s="10"/>
       <c r="CW39" s="10"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>66</v>
       </c>
@@ -35535,7 +35535,7 @@
       <c r="CV40" s="10"/>
       <c r="CW40" s="10"/>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>67</v>
       </c>
@@ -35766,7 +35766,7 @@
       <c r="CV41" s="10"/>
       <c r="CW41" s="10"/>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>68</v>
       </c>
@@ -35997,7 +35997,7 @@
       <c r="CV42" s="10"/>
       <c r="CW42" s="10"/>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>69</v>
       </c>
@@ -36228,7 +36228,7 @@
       <c r="CV43" s="10"/>
       <c r="CW43" s="10"/>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>70</v>
       </c>
@@ -36459,7 +36459,7 @@
       <c r="CV44" s="10"/>
       <c r="CW44" s="10"/>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>71</v>
       </c>
@@ -36690,7 +36690,7 @@
       <c r="CV45" s="10"/>
       <c r="CW45" s="10"/>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>72</v>
       </c>
@@ -36921,7 +36921,7 @@
       <c r="CV46" s="10"/>
       <c r="CW46" s="10"/>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>73</v>
       </c>
@@ -37152,7 +37152,7 @@
       <c r="CV47" s="10"/>
       <c r="CW47" s="10"/>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>74</v>
       </c>
@@ -37383,7 +37383,7 @@
       <c r="CV48" s="10"/>
       <c r="CW48" s="10"/>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>75</v>
       </c>
@@ -37614,7 +37614,7 @@
       <c r="CV49" s="10"/>
       <c r="CW49" s="10"/>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>76</v>
       </c>
@@ -37845,7 +37845,7 @@
       <c r="CV50" s="10"/>
       <c r="CW50" s="10"/>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>77</v>
       </c>
@@ -38076,7 +38076,7 @@
       <c r="CV51" s="10"/>
       <c r="CW51" s="10"/>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>78</v>
       </c>
@@ -38307,7 +38307,7 @@
       <c r="CV52" s="10"/>
       <c r="CW52" s="10"/>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>79</v>
       </c>
@@ -38538,7 +38538,7 @@
       <c r="CV53" s="10"/>
       <c r="CW53" s="10"/>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>80</v>
       </c>
@@ -38769,7 +38769,7 @@
       <c r="CV54" s="10"/>
       <c r="CW54" s="10"/>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>81</v>
       </c>
@@ -39000,7 +39000,7 @@
       <c r="CV55" s="10"/>
       <c r="CW55" s="10"/>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -39080,7 +39080,7 @@
       <c r="BZ56" s="9"/>
       <c r="CA56" s="9"/>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -39160,7 +39160,7 @@
       <c r="BZ57" s="9"/>
       <c r="CA57" s="9"/>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -39240,7 +39240,7 @@
       <c r="BZ58" s="9"/>
       <c r="CA58" s="9"/>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -39320,7 +39320,7 @@
       <c r="BZ59" s="9"/>
       <c r="CA59" s="9"/>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -39409,31 +39409,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CW60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="11" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="64" width="11.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="11" customWidth="1"/>
+    <col min="3" max="6" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="64" width="11.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="65" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -39627,7 +39627,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -39858,7 +39858,7 @@
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -40089,7 +40089,7 @@
       <c r="CV5" s="10"/>
       <c r="CW5" s="10"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -40320,7 +40320,7 @@
       <c r="CV6" s="10"/>
       <c r="CW6" s="10"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
@@ -40551,7 +40551,7 @@
       <c r="CV7" s="10"/>
       <c r="CW7" s="10"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -40782,7 +40782,7 @@
       <c r="CV8" s="10"/>
       <c r="CW8" s="10"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -41013,7 +41013,7 @@
       <c r="CV9" s="10"/>
       <c r="CW9" s="10"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -41244,7 +41244,7 @@
       <c r="CV10" s="10"/>
       <c r="CW10" s="10"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>37</v>
       </c>
@@ -41475,7 +41475,7 @@
       <c r="CV11" s="10"/>
       <c r="CW11" s="10"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
@@ -41706,7 +41706,7 @@
       <c r="CV12" s="10"/>
       <c r="CW12" s="10"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -41937,7 +41937,7 @@
       <c r="CV13" s="10"/>
       <c r="CW13" s="10"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>40</v>
       </c>
@@ -42168,7 +42168,7 @@
       <c r="CV14" s="10"/>
       <c r="CW14" s="10"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
@@ -42399,7 +42399,7 @@
       <c r="CV15" s="10"/>
       <c r="CW15" s="10"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -42630,7 +42630,7 @@
       <c r="CV16" s="10"/>
       <c r="CW16" s="10"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
@@ -42861,7 +42861,7 @@
       <c r="CV17" s="10"/>
       <c r="CW17" s="10"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>44</v>
       </c>
@@ -43092,7 +43092,7 @@
       <c r="CV18" s="10"/>
       <c r="CW18" s="10"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -43323,7 +43323,7 @@
       <c r="CV19" s="10"/>
       <c r="CW19" s="10"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -43554,7 +43554,7 @@
       <c r="CV20" s="10"/>
       <c r="CW20" s="10"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
@@ -43785,7 +43785,7 @@
       <c r="CV21" s="10"/>
       <c r="CW21" s="10"/>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
@@ -44016,7 +44016,7 @@
       <c r="CV22" s="10"/>
       <c r="CW22" s="10"/>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>49</v>
       </c>
@@ -44247,7 +44247,7 @@
       <c r="CV23" s="10"/>
       <c r="CW23" s="10"/>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
@@ -44478,7 +44478,7 @@
       <c r="CV24" s="10"/>
       <c r="CW24" s="10"/>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
@@ -44709,7 +44709,7 @@
       <c r="CV25" s="10"/>
       <c r="CW25" s="10"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>52</v>
       </c>
@@ -44940,7 +44940,7 @@
       <c r="CV26" s="10"/>
       <c r="CW26" s="10"/>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
@@ -45171,7 +45171,7 @@
       <c r="CV27" s="10"/>
       <c r="CW27" s="10"/>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>54</v>
       </c>
@@ -45402,7 +45402,7 @@
       <c r="CV28" s="10"/>
       <c r="CW28" s="10"/>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>55</v>
       </c>
@@ -45633,7 +45633,7 @@
       <c r="CV29" s="10"/>
       <c r="CW29" s="10"/>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>56</v>
       </c>
@@ -45864,7 +45864,7 @@
       <c r="CV30" s="10"/>
       <c r="CW30" s="10"/>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>57</v>
       </c>
@@ -46095,7 +46095,7 @@
       <c r="CV31" s="10"/>
       <c r="CW31" s="10"/>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>58</v>
       </c>
@@ -46326,7 +46326,7 @@
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>59</v>
       </c>
@@ -46557,7 +46557,7 @@
       <c r="CV33" s="10"/>
       <c r="CW33" s="10"/>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>60</v>
       </c>
@@ -46788,7 +46788,7 @@
       <c r="CV34" s="10"/>
       <c r="CW34" s="10"/>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>61</v>
       </c>
@@ -47019,7 +47019,7 @@
       <c r="CV35" s="10"/>
       <c r="CW35" s="10"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>62</v>
       </c>
@@ -47250,7 +47250,7 @@
       <c r="CV36" s="10"/>
       <c r="CW36" s="10"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
@@ -47481,7 +47481,7 @@
       <c r="CV37" s="10"/>
       <c r="CW37" s="10"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>64</v>
       </c>
@@ -47712,7 +47712,7 @@
       <c r="CV38" s="10"/>
       <c r="CW38" s="10"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -47943,7 +47943,7 @@
       <c r="CV39" s="10"/>
       <c r="CW39" s="10"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>66</v>
       </c>
@@ -48174,7 +48174,7 @@
       <c r="CV40" s="10"/>
       <c r="CW40" s="10"/>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>67</v>
       </c>
@@ -48405,7 +48405,7 @@
       <c r="CV41" s="10"/>
       <c r="CW41" s="10"/>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>68</v>
       </c>
@@ -48636,7 +48636,7 @@
       <c r="CV42" s="10"/>
       <c r="CW42" s="10"/>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>69</v>
       </c>
@@ -48867,7 +48867,7 @@
       <c r="CV43" s="10"/>
       <c r="CW43" s="10"/>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>70</v>
       </c>
@@ -49098,7 +49098,7 @@
       <c r="CV44" s="10"/>
       <c r="CW44" s="10"/>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>71</v>
       </c>
@@ -49329,7 +49329,7 @@
       <c r="CV45" s="10"/>
       <c r="CW45" s="10"/>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>72</v>
       </c>
@@ -49560,7 +49560,7 @@
       <c r="CV46" s="10"/>
       <c r="CW46" s="10"/>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>73</v>
       </c>
@@ -49791,7 +49791,7 @@
       <c r="CV47" s="10"/>
       <c r="CW47" s="10"/>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>74</v>
       </c>
@@ -50022,7 +50022,7 @@
       <c r="CV48" s="10"/>
       <c r="CW48" s="10"/>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>75</v>
       </c>
@@ -50253,7 +50253,7 @@
       <c r="CV49" s="10"/>
       <c r="CW49" s="10"/>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>76</v>
       </c>
@@ -50484,7 +50484,7 @@
       <c r="CV50" s="10"/>
       <c r="CW50" s="10"/>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>77</v>
       </c>
@@ -50715,7 +50715,7 @@
       <c r="CV51" s="10"/>
       <c r="CW51" s="10"/>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>78</v>
       </c>
@@ -50946,7 +50946,7 @@
       <c r="CV52" s="10"/>
       <c r="CW52" s="10"/>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>79</v>
       </c>
@@ -51177,7 +51177,7 @@
       <c r="CV53" s="10"/>
       <c r="CW53" s="10"/>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>80</v>
       </c>
@@ -51408,7 +51408,7 @@
       <c r="CV54" s="10"/>
       <c r="CW54" s="10"/>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>81</v>
       </c>
@@ -51639,7 +51639,7 @@
       <c r="CV55" s="10"/>
       <c r="CW55" s="10"/>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -51719,7 +51719,7 @@
       <c r="BZ56" s="9"/>
       <c r="CA56" s="9"/>
     </row>
-    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -51799,7 +51799,7 @@
       <c r="BZ57" s="9"/>
       <c r="CA57" s="9"/>
     </row>
-    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -51879,7 +51879,7 @@
       <c r="BZ58" s="9"/>
       <c r="CA58" s="9"/>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -51959,7 +51959,7 @@
       <c r="BZ59" s="9"/>
       <c r="CA59" s="9"/>
     </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -52041,5 +52041,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>